<commit_message>
Added link for video
</commit_message>
<xml_diff>
--- a/traffic_data.xlsx
+++ b/traffic_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -581,6 +581,24 @@
         <v>34</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Location 1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2024-12-13</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>24</v>
+      </c>
+      <c r="D9" t="n">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>